<commit_message>
Add test cases + Add readme.md
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginTestDataSet.xlsx
+++ b/src/test/resources/LoginTestDataSet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Standard_user</t>
   </si>
   <si>
+    <t>standard_user@</t>
+  </si>
+  <si>
     <t>Epic sadface: Username is required</t>
   </si>
   <si>
@@ -54,13 +57,22 @@
   </si>
   <si>
     <t>Secret_sauce</t>
+  </si>
+  <si>
+    <t>secret_sauce#</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>Epic sadface: Sorry, this user has been locked out.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -74,6 +86,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -93,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -101,6 +119,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -416,35 +437,35 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -467,6 +488,39 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>